<commit_message>
Add cruises 9 and 10 to data load
</commit_message>
<xml_diff>
--- a/data/biology/counts/08152019.xlsx
+++ b/data/biology/counts/08152019.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Desktop\Front Project and UCD\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E62497-65E8-4088-9BF8-0BE8DEF6044D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26122"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="260" windowWidth="19120" windowHeight="10540" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="311" sheetId="1" r:id="rId1"/>
@@ -20,12 +14,25 @@
     <sheet name="331" sheetId="4" r:id="rId5"/>
     <sheet name="332" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="67">
   <si>
     <t>date</t>
   </si>
@@ -63,12 +70,6 @@
     <t>bottom</t>
   </si>
   <si>
-    <t>b.improvisus</t>
-  </si>
-  <si>
-    <t>b.crenatus</t>
-  </si>
-  <si>
     <t>umbo</t>
   </si>
   <si>
@@ -84,9 +85,6 @@
     <t>chaetognath</t>
   </si>
   <si>
-    <t>m.californianus</t>
-  </si>
-  <si>
     <t>adult</t>
   </si>
   <si>
@@ -99,24 +97,15 @@
     <t>cyclopoid</t>
   </si>
   <si>
-    <t>metanaup</t>
-  </si>
-  <si>
     <t>embryo</t>
   </si>
   <si>
-    <t>zoea</t>
-  </si>
-  <si>
     <t>bivalve</t>
   </si>
   <si>
     <t>gastropod</t>
   </si>
   <si>
-    <t>harpacticoid</t>
-  </si>
-  <si>
     <t>phoronid</t>
   </si>
   <si>
@@ -132,27 +121,15 @@
     <t>larva</t>
   </si>
   <si>
-    <t>cyp</t>
-  </si>
-  <si>
     <t>diatom</t>
   </si>
   <si>
-    <t>naup4.5</t>
-  </si>
-  <si>
-    <t>naup2.3</t>
-  </si>
-  <si>
     <t>zoea1</t>
   </si>
   <si>
     <t>zoea2</t>
   </si>
   <si>
-    <t>zoea3</t>
-  </si>
-  <si>
     <t>egg.large</t>
   </si>
   <si>
@@ -174,12 +151,6 @@
     <t>actinotroch</t>
   </si>
   <si>
-    <t>cryptolithodes.sp</t>
-  </si>
-  <si>
-    <t>oikopleura.sp</t>
-  </si>
-  <si>
     <t>surface</t>
   </si>
   <si>
@@ -207,21 +178,12 @@
     <t>offshore</t>
   </si>
   <si>
-    <t>naup 4.5</t>
-  </si>
-  <si>
     <t>lithothidae</t>
   </si>
   <si>
-    <t>egg.invert</t>
-  </si>
-  <si>
     <t>setiger</t>
   </si>
   <si>
-    <t>setagers</t>
-  </si>
-  <si>
     <t>calyptopsis</t>
   </si>
   <si>
@@ -231,16 +193,52 @@
     <t>furcilia</t>
   </si>
   <si>
-    <t>euphausid</t>
-  </si>
-  <si>
-    <t>late.larva</t>
+    <t>chthamalus.spp</t>
+  </si>
+  <si>
+    <t>balanus.crenatus</t>
+  </si>
+  <si>
+    <t>nauplius4.5</t>
+  </si>
+  <si>
+    <t>nauplius2.3</t>
+  </si>
+  <si>
+    <t>cyprid</t>
+  </si>
+  <si>
+    <t>metanauplius</t>
+  </si>
+  <si>
+    <t>oikopleura</t>
+  </si>
+  <si>
+    <t>cryptolithodes.spp</t>
+  </si>
+  <si>
+    <t>zoea1.3</t>
+  </si>
+  <si>
+    <t>mytilus.spp</t>
+  </si>
+  <si>
+    <t>egg.invertebrate</t>
+  </si>
+  <si>
+    <t>nauplius 4.5</t>
+  </si>
+  <si>
+    <t>euphausiid</t>
+  </si>
+  <si>
+    <t>balanus.glandula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#\ ???/???"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
@@ -318,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -353,6 +351,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,31 +567,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" style="17" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" style="17" customWidth="1"/>
-    <col min="3" max="3" width="6.81640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" style="17" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" style="17" customWidth="1"/>
-    <col min="8" max="8" width="10.08984375" style="17" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" style="18" customWidth="1"/>
-    <col min="10" max="16384" width="14.453125" style="17"/>
+    <col min="1" max="1" width="11.1640625" style="17" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="17" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="17" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="17" customWidth="1"/>
+    <col min="9" max="9" width="8.5" style="18" customWidth="1"/>
+    <col min="10" max="16384" width="14.5" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -621,7 +621,7 @@
       </c>
       <c r="J1" s="13"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="6">
         <v>43692</v>
       </c>
@@ -641,17 +641,17 @@
         <v>64</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="I2" s="7">
-        <v>7</v>
+        <v>855</v>
       </c>
       <c r="J2" s="14"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="6">
         <v>43692</v>
       </c>
@@ -671,17 +671,17 @@
         <v>64</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I3" s="7">
-        <v>362</v>
+        <v>715</v>
       </c>
       <c r="J3" s="14"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" s="6">
         <v>43692</v>
       </c>
@@ -701,17 +701,17 @@
         <v>64</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="I4" s="7">
-        <v>58</v>
+        <v>562</v>
       </c>
       <c r="J4" s="14"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" s="6">
         <v>43692</v>
       </c>
@@ -731,17 +731,17 @@
         <v>64</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="I5" s="7">
-        <v>22</v>
+        <v>362</v>
       </c>
       <c r="J5" s="14"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="6">
         <v>43692</v>
       </c>
@@ -761,17 +761,17 @@
         <v>64</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I6" s="7">
-        <v>8</v>
+        <v>248</v>
       </c>
       <c r="J6" s="14"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
       <c r="A7" s="6">
         <v>43692</v>
       </c>
@@ -791,17 +791,17 @@
         <v>64</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I7" s="7">
-        <v>710</v>
+        <v>58</v>
       </c>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
       <c r="A8" s="6">
         <v>43692</v>
       </c>
@@ -821,17 +821,17 @@
         <v>64</v>
       </c>
       <c r="G8" s="14" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I8" s="7">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="J8" s="14"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="6">
         <v>43692</v>
       </c>
@@ -851,17 +851,17 @@
         <v>64</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I9" s="7">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="A10" s="6">
         <v>43692</v>
       </c>
@@ -881,17 +881,17 @@
         <v>64</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="I10" s="7">
-        <v>855</v>
+        <v>22</v>
       </c>
       <c r="J10" s="14"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="A11" s="6">
         <v>43692</v>
       </c>
@@ -911,17 +911,17 @@
         <v>64</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="I11" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="A12" s="6">
         <v>43692</v>
       </c>
@@ -941,17 +941,17 @@
         <v>64</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="I12" s="7">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="J12" s="14"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="6">
         <v>43692</v>
       </c>
@@ -971,17 +971,17 @@
         <v>64</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I13" s="7">
-        <v>248</v>
+        <v>9</v>
       </c>
       <c r="J13" s="14"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="6">
         <v>43692</v>
       </c>
@@ -1001,17 +1001,17 @@
         <v>64</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="I14" s="7">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J14" s="14"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
       <c r="A15" s="6">
         <v>43692</v>
       </c>
@@ -1031,17 +1031,17 @@
         <v>64</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="I15" s="7">
         <v>7</v>
       </c>
       <c r="J15" s="14"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="6">
         <v>43692</v>
       </c>
@@ -1061,17 +1061,17 @@
         <v>64</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="I16" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1">
       <c r="A17" s="6">
         <v>43692</v>
       </c>
@@ -1091,17 +1091,17 @@
         <v>64</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="I17" s="7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J17" s="14"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1">
       <c r="A18" s="6">
         <v>43692</v>
       </c>
@@ -1121,17 +1121,17 @@
         <v>64</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="I18" s="7">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="J18" s="14"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="6">
         <v>43692</v>
       </c>
@@ -1151,17 +1151,17 @@
         <v>64</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="I19" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J19" s="14"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1">
       <c r="A20" s="6">
         <v>43692</v>
       </c>
@@ -1181,17 +1181,17 @@
         <v>64</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="I20" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20" s="14"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="14">
       <c r="A21" s="6">
         <v>43692</v>
       </c>
@@ -1211,17 +1211,17 @@
         <v>64</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="I21" s="7">
         <v>1</v>
       </c>
       <c r="J21" s="14"/>
     </row>
-    <row r="22" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="14">
       <c r="A22" s="6">
         <v>43692</v>
       </c>
@@ -1241,17 +1241,17 @@
         <v>64</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="I22" s="7">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="J22" s="14"/>
     </row>
-    <row r="23" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="14">
       <c r="A23" s="6">
         <v>43692</v>
       </c>
@@ -1271,17 +1271,17 @@
         <v>64</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="I23" s="7">
         <v>1</v>
       </c>
       <c r="J23" s="14"/>
     </row>
-    <row r="24" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="14">
       <c r="A24" s="6">
         <v>43692</v>
       </c>
@@ -1301,17 +1301,17 @@
         <v>64</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I24" s="7">
-        <v>562</v>
+        <v>1</v>
       </c>
       <c r="J24" s="14"/>
     </row>
-    <row r="25" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1">
       <c r="A25" s="6">
         <v>43692</v>
       </c>
@@ -1328,20 +1328,19 @@
         <v>11</v>
       </c>
       <c r="F25" s="15">
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" s="7">
+        <v>15</v>
+      </c>
+      <c r="H25" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I25" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1">
       <c r="A26" s="6">
         <v>43692</v>
       </c>
@@ -1361,16 +1360,16 @@
         <v>16</v>
       </c>
       <c r="G26" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="17" t="s">
-        <v>20</v>
+        <v>63</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="I26" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1">
       <c r="A27" s="6">
         <v>43692</v>
       </c>
@@ -1390,16 +1389,16 @@
         <v>16</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="14" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="H27" s="17" t="s">
+        <v>17</v>
       </c>
       <c r="I27" s="18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" customHeight="1">
       <c r="A28" s="6">
         <v>43692</v>
       </c>
@@ -1419,77 +1418,59 @@
         <v>16</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I28" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6">
-        <v>43692</v>
-      </c>
-      <c r="B29" s="14">
-        <v>311</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F29" s="15">
-        <v>16</v>
-      </c>
-      <c r="G29" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H29" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="18">
-        <v>1</v>
-      </c>
+    <row r="30" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A30" s="20"/>
     </row>
   </sheetData>
+  <sortState ref="A2:J23">
+    <sortCondition descending="1" ref="I2:I23"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99DBC733-8A98-423C-8CE8-10C41DD5BA69}">
-  <dimension ref="A1:M27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="5.36328125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625" style="2"/>
-    <col min="6" max="6" width="6.26953125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.6640625" style="2"/>
+    <col min="6" max="6" width="6.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" style="2"/>
     <col min="10" max="10" width="11" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.08984375" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="2"/>
+    <col min="11" max="11" width="9.5" style="2" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1521,7 +1502,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13">
       <c r="A2" s="9">
         <v>43692</v>
       </c>
@@ -1535,23 +1516,22 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F2" s="11">
         <v>64</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2">
-        <v>35</v>
-      </c>
-      <c r="K2" s="12"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="9">
         <v>43692</v>
       </c>
@@ -1565,23 +1545,23 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F3" s="11">
         <v>64</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2">
-        <v>2</v>
+        <v>554</v>
       </c>
       <c r="K3" s="12"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13">
       <c r="A4" s="9">
         <v>43692</v>
       </c>
@@ -1595,23 +1575,22 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F4" s="11">
         <v>64</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="16" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="12"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="9">
         <v>43692</v>
       </c>
@@ -1625,23 +1604,22 @@
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F5" s="11">
         <v>64</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2">
-        <v>552</v>
-      </c>
-      <c r="K5" s="12"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="9">
         <v>43692</v>
       </c>
@@ -1655,23 +1633,22 @@
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F6" s="11">
         <v>64</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6" s="2">
-        <v>2</v>
-      </c>
-      <c r="K6" s="12"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="9">
         <v>43692</v>
       </c>
@@ -1685,22 +1662,22 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F7" s="11">
         <v>64</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="9">
         <v>43692</v>
       </c>
@@ -1714,22 +1691,23 @@
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F8" s="11">
         <v>64</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I8" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="K8" s="12"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="9">
         <v>43692</v>
       </c>
@@ -1743,22 +1721,22 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F9" s="11">
         <v>64</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I9" s="2">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="9">
         <v>43692</v>
       </c>
@@ -1772,22 +1750,22 @@
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F10" s="11">
         <v>64</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>20</v>
+        <v>42</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>36</v>
       </c>
       <c r="I10" s="2">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="9">
         <v>43692</v>
       </c>
@@ -1801,22 +1779,23 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F11" s="11">
         <v>64</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="9">
         <v>43692</v>
       </c>
@@ -1830,22 +1809,23 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F12" s="11">
         <v>64</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="I12" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="K12" s="12"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="9">
         <v>43692</v>
       </c>
@@ -1859,22 +1839,22 @@
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F13" s="11">
         <v>64</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>46</v>
+      <c r="G13" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="I13" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="9">
         <v>43692</v>
       </c>
@@ -1888,22 +1868,22 @@
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F14" s="11">
         <v>64</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="I14" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13">
       <c r="A15" s="9">
         <v>43692</v>
       </c>
@@ -1917,22 +1897,22 @@
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F15" s="11">
         <v>64</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="9">
         <v>43692</v>
       </c>
@@ -1946,22 +1926,23 @@
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F16" s="11">
         <v>64</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="I16" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="9">
         <v>43692</v>
       </c>
@@ -1975,22 +1956,22 @@
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F17" s="11">
         <v>64</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="I17" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="9">
         <v>43692</v>
       </c>
@@ -2004,22 +1985,22 @@
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F18" s="11">
         <v>64</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I18" s="2">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="9">
         <v>43692</v>
       </c>
@@ -2033,22 +2014,22 @@
         <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F19" s="11">
         <v>64</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="I19" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="9">
         <v>43692</v>
       </c>
@@ -2062,22 +2043,22 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F20" s="11">
         <v>8</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="9">
         <v>43692</v>
       </c>
@@ -2091,22 +2072,22 @@
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F21" s="11">
         <v>8</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="I21" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="9">
         <v>43692</v>
       </c>
@@ -2120,88 +2101,67 @@
         <v>10</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F22" s="11">
         <v>8</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="I22" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="9">
-        <v>43692</v>
-      </c>
-      <c r="B23" s="2">
-        <v>312</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F23" s="11">
-        <v>8</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I23" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
+      <c r="A23" s="9"/>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="21"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="9"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="9"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
-    </row>
   </sheetData>
+  <sortState ref="A1:M19">
+    <sortCondition descending="1" ref="I1:I19"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16024213-CD72-475A-9193-05D26CA60DA0}">
-  <dimension ref="A1:L21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="13.54296875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="8.6640625" style="2"/>
+    <col min="7" max="7" width="16.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="2" customWidth="1"/>
     <col min="9" max="9" width="10" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="2"/>
+    <col min="10" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2233,7 +2193,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="9">
         <v>43692</v>
       </c>
@@ -2244,7 +2204,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -2253,16 +2213,16 @@
         <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>60</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="9">
         <v>43692</v>
       </c>
@@ -2273,7 +2233,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
@@ -2282,16 +2242,16 @@
         <v>128</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="9">
         <v>43692</v>
       </c>
@@ -2302,7 +2262,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
@@ -2311,16 +2271,16 @@
         <v>128</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="9">
         <v>43692</v>
       </c>
@@ -2331,7 +2291,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -2340,16 +2300,16 @@
         <v>128</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="9">
         <v>43692</v>
       </c>
@@ -2360,7 +2320,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -2369,16 +2329,16 @@
         <v>128</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I6" s="2">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7" s="9">
         <v>43692</v>
       </c>
@@ -2389,7 +2349,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
@@ -2398,16 +2358,16 @@
         <v>128</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="I7" s="2">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="9">
         <v>43692</v>
       </c>
@@ -2418,7 +2378,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
@@ -2427,16 +2387,16 @@
         <v>128</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="I8" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="9">
         <v>43692</v>
       </c>
@@ -2447,7 +2407,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
@@ -2456,16 +2416,16 @@
         <v>128</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="I9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="9">
         <v>43692</v>
       </c>
@@ -2476,7 +2436,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
@@ -2485,16 +2445,16 @@
         <v>128</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I10" s="2">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="9">
         <v>43692</v>
       </c>
@@ -2505,7 +2465,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
@@ -2514,16 +2474,16 @@
         <v>128</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="9">
         <v>43692</v>
       </c>
@@ -2534,7 +2494,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
@@ -2543,16 +2503,16 @@
         <v>128</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="I12" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="9">
         <v>43692</v>
       </c>
@@ -2563,7 +2523,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
@@ -2572,16 +2532,16 @@
         <v>128</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="I13" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="9">
         <v>43692</v>
       </c>
@@ -2592,25 +2552,25 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="2">
-        <v>128</v>
+      <c r="F14" s="10">
+        <v>32</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I14" s="2">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="9">
         <v>43692</v>
       </c>
@@ -2621,7 +2581,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>11</v>
@@ -2630,16 +2590,16 @@
         <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="I15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="9">
         <v>43692</v>
       </c>
@@ -2650,7 +2610,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>11</v>
@@ -2659,81 +2619,60 @@
         <v>32</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="I16" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
-        <v>43692</v>
-      </c>
-      <c r="B17" s="2">
-        <v>321</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="10">
-        <v>32</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
+      <c r="A17" s="9"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="21"/>
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1">
       <c r="A20" s="9"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-    </row>
   </sheetData>
+  <sortState ref="A1:L13">
+    <sortCondition descending="1" ref="I1:I13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1C8994-5FA5-4413-96B5-0503144D2B80}">
-  <dimension ref="A1:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.36328125" style="2" customWidth="1"/>
-    <col min="2" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="13.36328125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="10.5" style="2" customWidth="1"/>
+    <col min="2" max="6" width="8.6640625" style="2"/>
+    <col min="7" max="7" width="17" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2765,7 +2704,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="9">
         <v>43692</v>
       </c>
@@ -2776,25 +2715,25 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2">
         <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="9">
         <v>43692</v>
       </c>
@@ -2805,25 +2744,25 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F3" s="2">
         <v>128</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="9">
         <v>43692</v>
       </c>
@@ -2834,25 +2773,25 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2">
         <v>128</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="9">
         <v>43692</v>
       </c>
@@ -2863,25 +2802,25 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2">
         <v>128</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="9">
         <v>43692</v>
       </c>
@@ -2892,25 +2831,25 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F6" s="2">
         <v>128</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="9">
         <v>43692</v>
       </c>
@@ -2921,25 +2860,25 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
         <v>128</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I7" s="2">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="9">
         <v>43692</v>
       </c>
@@ -2950,25 +2889,25 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F8" s="2">
         <v>128</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="I8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="9">
         <v>43692</v>
       </c>
@@ -2979,25 +2918,25 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2">
         <v>128</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="I9" s="2">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="9">
         <v>43692</v>
       </c>
@@ -3008,25 +2947,25 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F10" s="2">
         <v>128</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I10" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="9">
         <v>43692</v>
       </c>
@@ -3037,25 +2976,25 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F11" s="2">
         <v>128</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="I11" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="9">
         <v>43692</v>
       </c>
@@ -3066,25 +3005,25 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2">
         <v>128</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="I12" s="2">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="9">
         <v>43692</v>
       </c>
@@ -3095,25 +3034,25 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2">
         <v>128</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="I13" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14" s="9">
         <v>43692</v>
       </c>
@@ -3124,25 +3063,25 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F14" s="2">
         <v>32</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I14" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" s="9">
         <v>43692</v>
       </c>
@@ -3153,25 +3092,25 @@
         <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2">
         <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="I15" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" s="9">
         <v>43692</v>
       </c>
@@ -3182,26 +3121,26 @@
         <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F16" s="2">
         <v>32</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="I16" s="2">
         <v>1</v>
       </c>
       <c r="J16" s="16"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="9">
         <v>43692</v>
       </c>
@@ -3212,25 +3151,25 @@
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F17" s="2">
         <v>32</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="I17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="9">
         <v>43692</v>
       </c>
@@ -3241,48 +3180,59 @@
         <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2">
         <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="I18" s="2">
         <v>1</v>
       </c>
     </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1"/>
+    </row>
   </sheetData>
+  <sortState ref="A1:L13">
+    <sortCondition descending="1" ref="I1:I13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464DC4D1-82F0-484E-B5E5-DA1D0F42F821}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.08984375" style="2" customWidth="1"/>
-    <col min="2" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="12.90625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" style="2" customWidth="1"/>
+    <col min="2" max="6" width="8.6640625" style="2"/>
+    <col min="7" max="7" width="18.5" style="2" customWidth="1"/>
     <col min="8" max="8" width="11" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="9" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3314,7 +3264,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="9">
         <v>43692</v>
       </c>
@@ -3325,7 +3275,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -3334,16 +3284,16 @@
         <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="9">
         <v>43692</v>
       </c>
@@ -3354,7 +3304,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
@@ -3366,13 +3316,13 @@
         <v>13</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="9">
         <v>43692</v>
       </c>
@@ -3383,7 +3333,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
@@ -3392,16 +3342,16 @@
         <v>128</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="9">
         <v>43692</v>
       </c>
@@ -3412,7 +3362,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -3421,16 +3371,16 @@
         <v>128</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="9">
         <v>43692</v>
       </c>
@@ -3441,25 +3391,25 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2">
+        <v>128</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2">
-        <v>128</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="9">
         <v>43692</v>
       </c>
@@ -3470,7 +3420,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
@@ -3479,16 +3429,16 @@
         <v>128</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="I7" s="2">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="9">
         <v>43692</v>
       </c>
@@ -3499,7 +3449,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
@@ -3508,16 +3458,16 @@
         <v>128</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="I8" s="2">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="9">
         <v>43692</v>
       </c>
@@ -3528,7 +3478,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
@@ -3537,16 +3487,16 @@
         <v>128</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I9" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="9">
         <v>43692</v>
       </c>
@@ -3557,7 +3507,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
@@ -3566,16 +3516,16 @@
         <v>128</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="I10" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="9">
         <v>43692</v>
       </c>
@@ -3586,7 +3536,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
@@ -3595,16 +3545,16 @@
         <v>128</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="I11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="9">
         <v>43692</v>
       </c>
@@ -3615,7 +3565,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
@@ -3624,16 +3574,16 @@
         <v>128</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="I12" s="2">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1">
       <c r="A13" s="9">
         <v>43692</v>
       </c>
@@ -3644,7 +3594,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
@@ -3653,16 +3603,16 @@
         <v>128</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="I13" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:12" ht="15" thickBot="1">
       <c r="A14" s="9">
         <v>43692</v>
       </c>
@@ -3673,7 +3623,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
@@ -3682,16 +3632,16 @@
         <v>32</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I14" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:12" ht="15" thickBot="1">
       <c r="A15" s="9">
         <v>43692</v>
       </c>
@@ -3702,7 +3652,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>11</v>
@@ -3711,16 +3661,16 @@
         <v>32</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I15" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:12" ht="15" thickBot="1">
       <c r="A16" s="9">
         <v>43692</v>
       </c>
@@ -3731,7 +3681,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>11</v>
@@ -3740,51 +3690,59 @@
         <v>32</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="I16" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1">
       <c r="A17" s="9"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="9"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1">
+      <c r="A18" s="21"/>
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" s="9"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1">
       <c r="A20" s="9"/>
     </row>
   </sheetData>
+  <sortState ref="A1:L13">
+    <sortCondition descending="1" ref="I1:I13"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4CC8FC4-F093-4F35-B229-8E9C7F3BEA9B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.453125" style="2" customWidth="1"/>
-    <col min="2" max="6" width="8.7265625" style="2"/>
-    <col min="7" max="7" width="13.54296875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.54296875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="10.5" style="2" customWidth="1"/>
+    <col min="2" max="6" width="8.6640625" style="2"/>
+    <col min="7" max="7" width="17.5" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3816,7 +3774,7 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="9">
         <v>43692</v>
       </c>
@@ -3827,25 +3785,25 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2">
         <v>128</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I2" s="2">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="9">
         <v>43692</v>
       </c>
@@ -3856,25 +3814,25 @@
         <v>9</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F3" s="2">
         <v>128</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="9">
         <v>43692</v>
       </c>
@@ -3885,25 +3843,25 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2">
         <v>128</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="9">
         <v>43692</v>
       </c>
@@ -3914,25 +3872,25 @@
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2">
         <v>128</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I5" s="2">
-        <v>878</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="9">
         <v>43692</v>
       </c>
@@ -3943,25 +3901,25 @@
         <v>9</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2">
+        <v>128</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="2">
-        <v>128</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="9">
         <v>43692</v>
       </c>
@@ -3972,25 +3930,25 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2">
         <v>128</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="I7" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="9">
         <v>43692</v>
       </c>
@@ -4001,25 +3959,25 @@
         <v>9</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F8" s="2">
         <v>128</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="I8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="9">
         <v>43692</v>
       </c>
@@ -4030,25 +3988,25 @@
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F9" s="2">
         <v>128</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="I9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="9">
         <v>43692</v>
       </c>
@@ -4059,25 +4017,25 @@
         <v>9</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F10" s="2">
         <v>128</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="I10" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="9">
         <v>43692</v>
       </c>
@@ -4088,25 +4046,25 @@
         <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F11" s="2">
         <v>128</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="I11" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="9">
         <v>43692</v>
       </c>
@@ -4117,25 +4075,25 @@
         <v>9</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F12" s="2">
         <v>128</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="I12" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="9">
         <v>43692</v>
       </c>
@@ -4146,25 +4104,25 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F13" s="2">
         <v>128</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="9">
         <v>43692</v>
       </c>
@@ -4175,25 +4133,25 @@
         <v>9</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="2">
+        <v>128</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="2">
-        <v>128</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="H14" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I14" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" s="9">
         <v>43692</v>
       </c>
@@ -4204,25 +4162,25 @@
         <v>9</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F15" s="2">
         <v>32</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="I15" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" s="9">
         <v>43692</v>
       </c>
@@ -4233,25 +4191,25 @@
         <v>9</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F16" s="2">
         <v>32</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="I16" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="9">
         <v>43692</v>
       </c>
@@ -4262,25 +4220,25 @@
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F17" s="2">
         <v>32</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="9">
         <v>43692</v>
       </c>
@@ -4291,32 +4249,40 @@
         <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F18" s="2">
         <v>32</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="I18" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="9"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="9"/>
+    <row r="20" spans="1:9">
+      <c r="A20" s="21"/>
     </row>
   </sheetData>
+  <sortState ref="A1:L14">
+    <sortCondition descending="1" ref="I1:I14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup orientation="landscape"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>